<commit_message>
Show AnkiForum posts count
</commit_message>
<xml_diff>
--- a/tests/anki_addons_dataset/exporter/xlsx/exp_data.xlsx
+++ b/tests/anki_addons_dataset/exporter/xlsx/exp_data.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -11,7 +11,7 @@
     <sheet name="Addons" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Addons!$A$2:$P$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Addons!$A$2:$Q$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -28,7 +28,7 @@
     <author>Unknown Author</author>
   </authors>
   <commentList>
-    <comment ref="O2" authorId="0">
+    <comment ref="P2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -40,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P2" authorId="0">
+    <comment ref="Q2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t xml:space="preserve">Anki Web</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t xml:space="preserve">Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Posts Count</t>
   </si>
   <si>
     <t xml:space="preserve">Last post</t>
@@ -228,16 +231,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -459,162 +466,170 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
+      <selection pane="bottomLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="80.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="6.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="50.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="80.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="6.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="12.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="50.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="10.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1" t="s">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="3" t="s">
         <v>17</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>1188705668</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="0" t="s">
+      <c r="H3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="0" t="n">
+      <c r="I3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="M3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3" s="0" t="n">
+      <c r="N3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="P3" s="0" t="n">
+      <c r="Q3" s="1" t="n">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:P2"/>
+  <autoFilter ref="A2:Q2"/>
   <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:P1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:Q1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H3" r:id="rId2" display="link"/>
     <hyperlink ref="I3" r:id="rId3" display="link"/>
-    <hyperlink ref="K3" r:id="rId4" display="link"/>
+    <hyperlink ref="L3" r:id="rId4" display="link"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>